<commit_message>
integration doc for GetDistancesAndSortByLimitingFactor
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_sortByLimitingFactor.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_sortByLimitingFactor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irish\Documents\SUM23-SFT221-NAA-4\Documents\Testing\TestsDocuments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/intaechung/Documents/Seneca/Semester 2/sft221/SUM23-SFT221-NAA-4/Documents/Testing/TestsDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BA409A-4E82-4CA0-BA75-97A9DE22F65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF34D044-014D-B243-9DFC-2276E849437B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5580" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -520,6 +520,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -560,11 +566,11 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -849,144 +855,144 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
-    </row>
-    <row r="3" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="23" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="25"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="31">
         <v>4</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="30"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="32"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="32"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="37"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="32"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="34"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+    <row r="12" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1013,28 +1019,28 @@
       <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
     <col min="3" max="3" width="65.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="56.109375" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="56.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="19"/>
       <c r="D1" s="16"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-    </row>
-    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>48</v>
       </c>
@@ -1076,11 +1082,11 @@
       <c r="F3" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>49</v>
       </c>
@@ -1099,11 +1105,11 @@
       <c r="F4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>50</v>
       </c>
@@ -1122,11 +1128,11 @@
       <c r="F5" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>51</v>
       </c>
@@ -1145,11 +1151,11 @@
       <c r="F6" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>52</v>
       </c>
@@ -1168,122 +1174,122 @@
       <c r="F7" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E45" s="3"/>
     </row>
   </sheetData>
@@ -1299,32 +1305,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DBEBE5-E65B-48FE-ACB2-E1CF3882866A}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="96" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
     <col min="3" max="3" width="65.33203125" customWidth="1"/>
     <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="56.109375" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" customWidth="1"/>
+    <col min="5" max="5" width="56.1640625" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-    </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1347,7 +1353,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>53</v>
       </c>
@@ -1366,11 +1372,11 @@
       <c r="F3" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
@@ -1389,11 +1395,11 @@
       <c r="F4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>55</v>
       </c>
@@ -1412,11 +1418,11 @@
       <c r="F5" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>56</v>
       </c>
@@ -1435,125 +1441,125 @@
       <c r="F6" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E45" s="3"/>
     </row>
   </sheetData>
@@ -1565,12 +1571,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1745,15 +1748,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1778,18 +1793,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>